<commit_message>
updated results with new graph
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin Xu\Desktop\cs224w\CS224W-Youtube-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF9D357-6340-499D-93AD-D2A3CF4F93A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA4E8CD-ADF1-4D55-8EE5-1AA299DA4D8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{2D893DD8-DCCB-4A3F-8D0F-CF42E5F1F960}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="20">
   <si>
     <t>random forest</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Rolx + genre</t>
+  </si>
+  <si>
+    <t>5 roles</t>
+  </si>
+  <si>
+    <t>3 roles</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1840FC73-C6A7-43B2-B74F-1E7CCC434545}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1158,484 +1164,881 @@
     <col min="3" max="3" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>0.95384615384615301</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>0.94709851551956803</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>0.94709851551956803</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>0.94709851551956803</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>0.98155645524066504</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="2">
         <v>0.85659019343229803</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.94035087719298205</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.94673864147548303</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.94673864147548303</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.94673864147548303</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.97903733693207295</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.89185784975258597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <v>0.91505216095380004</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>0.90608552631578898</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="2">
         <v>0.90608552631578898</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="2">
         <v>0.90608552631578898</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="2">
         <v>0.96471615720523995</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G4" s="2">
         <v>0.803770086526576</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.89287445467765303</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.90602369980250097</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.90602369980250097</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.90602369980250097</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.95970123328122203</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.82134363852556402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
         <v>0.99692363373145099</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>0.99692363373145099</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>0.99692363373145099</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>0.999457111834962</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G5" s="2">
         <v>0.94136807817589496</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="I5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.99619978284473398</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.99619978284473398</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.99619978284473398</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.99981903727832</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>0.95564202334630299</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>0.94933655006031303</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>0.94933655006031303</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="4">
         <v>0.94933655006031303</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
         <v>0.98177939738689801</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="4">
         <v>0.86714452408734699</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="I6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.94340588988476304</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.94897431477331395</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.94897431477331395</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.94897431477331395</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.97934946379508903</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0.90190958054512804</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>0.95501979129183101</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>0.94710327455919396</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>0.94710327455919396</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>0.94710327455919396</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>0.97445124145376005</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G7" s="2">
         <v>0.85606333213386099</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="I7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.94998200791651599</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.95645915797049297</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.95645915797049297</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.95645915797049297</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.97948902482907496</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.90248290752069005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
         <v>0.91914618369987</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>0.90938303341902305</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>0.90938303341902305</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>0.90938303341902305</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>0.95669824086603505</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>0.81033434650455904</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.91089743589743499</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.92483660130718903</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.92483660130718903</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.92483660130718903</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.96331521739130399</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.83983451536642995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
         <v>0.99577762139338499</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>0.99577762139338499</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>0.99577762139338499</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>0.99507389162561499</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>0.93807178043631201</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.99577762139338499</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.99577762139338499</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.99577762139338499</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.997888810696692</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>0.95786990225817303</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>0.95062143097077501</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>0.95062143097077501</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E10" s="2">
         <v>0.95062143097077501</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>0.97550879613659802</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>0.86953685583822504</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="I10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.95337135189533695</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.95899695018637698</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.95899695018637698</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.95899695018637698</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.98029726927065297</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.91294571153228399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="I12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
         <v>0.94871794871794801</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C13" s="2">
         <v>0.94817813765182102</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <v>0.94817813765182102</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E13" s="2">
         <v>0.94817813765182102</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>0.980026990553306</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <v>0.74062078272604503</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="I13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.94871794871794801</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.94817813765182102</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.94817813765182102</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.94817813765182102</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.980026990553306</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.74062078272604503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>0.90716398291160005</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C14" s="2">
         <v>0.91003976143141097</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>0.91003976143141097</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <v>0.91003976143141097</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <v>0.96137787056367396</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <v>0.75137911356286802</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.90716398291160005</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.91003976143141097</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.91003976143141097</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.91003976143141097</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.96137787056367396</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.75137911356286802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
         <v>0.999095186391603</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>0.99402823018458197</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="2">
         <v>0.99402823018458197</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="2">
         <v>0.99402823018458197</v>
       </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
         <v>0.71480275063336896</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="I15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.999095186391603</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.99402823018458197</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.99402823018458197</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.99402823018458197</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.71480275063336896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B16" s="4">
         <v>0.95091284877712701</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C16" s="4">
         <v>0.95018162947586904</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D16" s="4">
         <v>0.95018162947586904</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E16" s="4">
         <v>0.95018162947586904</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F16" s="4">
         <v>0.98030867482703499</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="4">
         <v>0.73263470277288301</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="I16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.95091284877712701</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.95018162947586904</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.95018162947586904</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.95018162947586904</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.98030867482703499</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0.73263470277288301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>0.94494422454120097</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>0.94710327455919396</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <v>0.94710327455919396</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <v>0.94710327455919396</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>0.97409139978409498</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>0.72148254767902098</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="I17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.94494422454120097</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.94710327455919396</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.94710327455919396</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.94710327455919396</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.97409139978409498</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.72148254767902098</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>0.90382165605095499</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>0.90990990990990905</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>0.90990990990990905</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E18" s="2">
         <v>0.90990990990990905</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>0.953597848016139</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G18" s="2">
         <v>0.74378296910324004</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="I18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.90382165605095499</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.953597848016139</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.74378296910324004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>0.998592540464461</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>0.99507389162561499</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>0.99507389162561499</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <v>0.99507389162561499</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>0.997888810696692</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G19" s="2">
         <v>0.69458128078817705</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="I19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.998592540464461</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.99507389162561499</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.99507389162561499</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.99507389162561499</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.997888810696692</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.69458128078817705</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="2">
         <v>0.94884653961885601</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <v>0.95058823529411696</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>0.95058823529411696</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <v>0.95058823529411696</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>0.97524071526822498</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G20" s="2">
         <v>0.71834061135371097</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="I20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.94884653961885601</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.95058823529411696</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.95058823529411696</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.95058823529411696</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0.97524071526822498</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.71834061135371097</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="I22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
         <v>0.944489428699955</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.497165991902834</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.497165991902834</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.497165991902834</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.92910481331533901</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0.738371569950517</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0.89982081772275602</v>
       </c>
       <c r="C23" s="2">
         <v>0.497165991902834</v>
@@ -1647,87 +2050,171 @@
         <v>0.497165991902834</v>
       </c>
       <c r="F23" s="2">
+        <v>0.92910481331533901</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.738371569950517</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.929284750337381</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.92460638776428195</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.89158794421952303</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.89982081772275602</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="F24" s="2">
         <v>0.89040870138431105</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>0.748481397114654</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="I24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.87883631713554899</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.497165991902834</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0.88363338788870704</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0.82289642803766205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B25" s="10">
         <v>0.999638074556641</v>
       </c>
-      <c r="C24" s="10">
-        <v>1</v>
-      </c>
-      <c r="D24" s="10">
-        <v>1</v>
-      </c>
-      <c r="E24" s="10">
-        <v>1</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="C25" s="10">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
         <v>0.97774158523344101</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G25" s="10">
         <v>0.71353601158161395</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="I25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="10">
+        <v>0.99493304379297798</v>
+      </c>
+      <c r="K25" s="10">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10">
+        <v>1</v>
+      </c>
+      <c r="M25" s="10">
+        <v>1</v>
+      </c>
+      <c r="N25" s="10">
+        <v>0.97701773434672401</v>
+      </c>
+      <c r="O25" s="10">
+        <v>0.99638074556641298</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B26" s="4">
         <v>0.94710672953278996</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C26" s="4">
         <v>0.664142779881016</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D26" s="4">
         <v>0.664142779881016</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E26" s="4">
         <v>0.664142779881016</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F26" s="4">
         <v>0.932033810591685</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G26" s="4">
         <v>0.73059106911246996</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="I26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.93328806654218199</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0.664142779881016</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0.664142779881016</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0.664142779881016</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0.92798212444138795</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0.90136694769583303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <v>0.94386469953220498</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0.51133501259445802</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.51133501259445802</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.51133501259445802</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.83807124865059301</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.72544080604534</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.90107799619530704</v>
       </c>
       <c r="C27" s="2">
         <v>0.51133501259445802</v>
@@ -1739,56 +2226,163 @@
         <v>0.51133501259445802</v>
       </c>
       <c r="F27" s="2">
+        <v>0.83807124865059301</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.72544080604534</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.92839150773659496</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0.83267362360561303</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0.88377114069809204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.90107799619530704</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="F28" s="2">
         <v>0.81794368041912202</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G28" s="2">
         <v>0.75114503816793898</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="I28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.87997512437810899</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.51133501259445802</v>
+      </c>
+      <c r="N28" s="2">
+        <v>0.81241830065359399</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0.81807647740440304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
         <v>0.87895847994370102</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G29" s="2">
         <v>0.69247009148486904</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="I29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.99577762139338499</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0.87473610133708601</v>
+      </c>
+      <c r="O29" s="2">
+        <v>0.99366643209007699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B30" s="11">
         <v>0.94796531020680397</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C30" s="11">
         <v>0.67666666666666597</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D30" s="11">
         <v>0.67666666666666597</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E30" s="11">
         <v>0.67666666666666597</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F30" s="11">
         <v>0.84735413839891405</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G30" s="11">
         <v>0.72061515928231401</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="11">
+        <v>0.934301749752393</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0.67666666666666597</v>
+      </c>
+      <c r="L30" s="11">
+        <v>0.67666666666666597</v>
+      </c>
+      <c r="M30" s="11">
+        <v>0.67666666666666597</v>
+      </c>
+      <c r="N30" s="11">
+        <v>0.84242629617078901</v>
+      </c>
+      <c r="O30" s="11">
+        <v>0.89736256752462595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added val and real test
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin Xu\Desktop\cs224w\CS224W-Youtube-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA4E8CD-ADF1-4D55-8EE5-1AA299DA4D8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43333C6C-FFF6-4896-9786-C7CA3E622346}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{2D893DD8-DCCB-4A3F-8D0F-CF42E5F1F960}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="2" xr2:uid="{2D893DD8-DCCB-4A3F-8D0F-CF42E5F1F960}"/>
   </bookViews>
   <sheets>
     <sheet name="unbalanced test" sheetId="1" r:id="rId1"/>
     <sheet name="balanced test" sheetId="2" r:id="rId2"/>
+    <sheet name="real, unbalanced test" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="24">
   <si>
     <t>random forest</t>
   </si>
@@ -91,6 +92,18 @@
   </si>
   <si>
     <t>3 roles</t>
+  </si>
+  <si>
+    <t>Val acc</t>
+  </si>
+  <si>
+    <t>Val precision</t>
+  </si>
+  <si>
+    <t>Val recall</t>
+  </si>
+  <si>
+    <t>Val F1</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1840FC73-C6A7-43B2-B74F-1E7CCC434545}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1647,22 +1660,22 @@
         <v>1</v>
       </c>
       <c r="J13" s="2">
-        <v>0.94871794871794801</v>
+        <v>0.93333333333333302</v>
       </c>
       <c r="K13" s="2">
-        <v>0.94817813765182102</v>
+        <v>0.95024741340530805</v>
       </c>
       <c r="L13" s="2">
-        <v>0.94817813765182102</v>
+        <v>0.95024741340530805</v>
       </c>
       <c r="M13" s="2">
-        <v>0.94817813765182102</v>
+        <v>0.95024741340530805</v>
       </c>
       <c r="N13" s="2">
-        <v>0.980026990553306</v>
+        <v>0.98110661268555999</v>
       </c>
       <c r="O13" s="2">
-        <v>0.74062078272604503</v>
+        <v>0.89302744039586102</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1691,22 +1704,22 @@
         <v>2</v>
       </c>
       <c r="J14" s="2">
-        <v>0.90716398291160005</v>
+        <v>0.882249560632688</v>
       </c>
       <c r="K14" s="2">
-        <v>0.91003976143141097</v>
+        <v>0.91187675998012196</v>
       </c>
       <c r="L14" s="2">
-        <v>0.91003976143141097</v>
+        <v>0.91187675998012196</v>
       </c>
       <c r="M14" s="2">
-        <v>0.91003976143141097</v>
+        <v>0.91187675998012196</v>
       </c>
       <c r="N14" s="2">
-        <v>0.96137787056367396</v>
+        <v>0.96355074991279999</v>
       </c>
       <c r="O14" s="2">
-        <v>0.75137911356286802</v>
+        <v>0.82293373045420704</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1735,22 +1748,22 @@
         <v>3</v>
       </c>
       <c r="J15" s="2">
-        <v>0.999095186391603</v>
+        <v>0.999276149113282</v>
       </c>
       <c r="K15" s="2">
-        <v>0.99402823018458197</v>
+        <v>0.99619978284473398</v>
       </c>
       <c r="L15" s="2">
-        <v>0.99402823018458197</v>
+        <v>0.99619978284473398</v>
       </c>
       <c r="M15" s="2">
-        <v>0.99402823018458197</v>
+        <v>0.99619978284473398</v>
       </c>
       <c r="N15" s="2">
-        <v>1</v>
+        <v>0.99981903727832</v>
       </c>
       <c r="O15" s="2">
-        <v>0.71480275063336896</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1779,22 +1792,22 @@
         <v>4</v>
       </c>
       <c r="J16" s="4">
-        <v>0.95091284877712701</v>
+        <v>0.93712346202800101</v>
       </c>
       <c r="K16" s="4">
-        <v>0.95018162947586904</v>
+        <v>0.95217504107930395</v>
       </c>
       <c r="L16" s="4">
-        <v>0.95018162947586904</v>
+        <v>0.95217504107930395</v>
       </c>
       <c r="M16" s="4">
-        <v>0.95018162947586904</v>
+        <v>0.95217504107930395</v>
       </c>
       <c r="N16" s="4">
-        <v>0.98030867482703499</v>
+        <v>0.98134991119005299</v>
       </c>
       <c r="O16" s="4">
-        <v>0.73263470277288301</v>
+        <v>0.90286741279307203</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1823,22 +1836,22 @@
         <v>16</v>
       </c>
       <c r="J17" s="2">
-        <v>0.94494422454120097</v>
+        <v>0.93558834112990197</v>
       </c>
       <c r="K17" s="2">
-        <v>0.94710327455919396</v>
+        <v>0.95609931630082701</v>
       </c>
       <c r="L17" s="2">
-        <v>0.94710327455919396</v>
+        <v>0.95609931630082701</v>
       </c>
       <c r="M17" s="2">
-        <v>0.94710327455919396</v>
+        <v>0.95609931630082701</v>
       </c>
       <c r="N17" s="2">
-        <v>0.97409139978409498</v>
+        <v>0.98128823317740199</v>
       </c>
       <c r="O17" s="2">
-        <v>0.72148254767902098</v>
+        <v>0.89528607412738304</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1867,22 +1880,22 @@
         <v>5</v>
       </c>
       <c r="J18" s="2">
-        <v>0.90382165605095499</v>
+        <v>0.88909774436090205</v>
       </c>
       <c r="K18" s="2">
-        <v>0.90990990990990905</v>
+        <v>0.92147955872809795</v>
       </c>
       <c r="L18" s="2">
-        <v>0.90990990990990905</v>
+        <v>0.92147955872809795</v>
       </c>
       <c r="M18" s="2">
-        <v>0.90990990990990905</v>
+        <v>0.92147955872809795</v>
       </c>
       <c r="N18" s="2">
-        <v>0.953597848016139</v>
+        <v>0.96723549488054605</v>
       </c>
       <c r="O18" s="2">
-        <v>0.74378296910324004</v>
+        <v>0.83002336448598102</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1914,19 +1927,19 @@
         <v>0.998592540464461</v>
       </c>
       <c r="K19" s="2">
-        <v>0.99507389162561499</v>
+        <v>0.99929627023223</v>
       </c>
       <c r="L19" s="2">
-        <v>0.99507389162561499</v>
+        <v>0.99929627023223</v>
       </c>
       <c r="M19" s="2">
-        <v>0.99507389162561499</v>
+        <v>0.99929627023223</v>
       </c>
       <c r="N19" s="2">
-        <v>0.997888810696692</v>
+        <v>0.997185080928923</v>
       </c>
       <c r="O19" s="2">
-        <v>0.69458128078817705</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1955,22 +1968,22 @@
         <v>6</v>
       </c>
       <c r="J20" s="2">
-        <v>0.94884653961885601</v>
+        <v>0.94066953927742802</v>
       </c>
       <c r="K20" s="2">
-        <v>0.95058823529411696</v>
+        <v>0.95881161377447599</v>
       </c>
       <c r="L20" s="2">
-        <v>0.95058823529411696</v>
+        <v>0.95881161377447599</v>
       </c>
       <c r="M20" s="2">
-        <v>0.95058823529411696</v>
+        <v>0.95881161377447599</v>
       </c>
       <c r="N20" s="2">
-        <v>0.97524071526822498</v>
+        <v>0.98198198198198094</v>
       </c>
       <c r="O20" s="2">
-        <v>0.71834061135371097</v>
+        <v>0.90711777848707298</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2388,4 +2401,951 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA978AED-DA6C-4084-9007-FE0533C5B64D}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.60325330132052801</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.58256902761104401</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.58256902761104401</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.58256902761104401</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.95894357743097203</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.52734693877550998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.71576940444533599</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.61597086396438905</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.61597086396438905</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.61597086396438905</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.92481553915903603</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.52036474164133695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.34252100840336103</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.43855942376950702</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.43855942376950702</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.43855942376950702</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.99911164465786295</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.69877551020408102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.463324726782611</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.51234152361718799</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.51234152361718799</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.51234152361718799</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.96052904923481697</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.59651567944250805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.86069183506765601</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.72766985119153305</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.72766985119153305</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.72766985119153305</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.85617253258514703</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.35874738075789298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1.0529695024076999E-2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>7.1090820153269204E-3</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7.1090820153269204E-3</v>
+      </c>
+      <c r="E8" s="10">
+        <v>7.1090820153269204E-3</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2.5421686746987901E-2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>4.40498218674915E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.37020316027088002</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.49209932279909702</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.49209932279909702</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.49209932279909702</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.95259593679458199</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.720090293453724</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.0476963416156801E-2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.4015687283014E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.4015687283014E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.4015687283014E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4.9521797805550598E-2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>8.7563991710242796E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.74880659665367</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.88089434580161996</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.88089434580161996</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.88089434580161996</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.86233325688440299</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.24621711140386901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.3161920951976201E-3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.9717682020802298E-3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.9717682020802298E-3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.9717682020802298E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.1710973181871399E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.7658859096431399E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.429133858267716</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.118110236220472</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.98425196850393704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.6075157458680301E-3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5.8763299648310497E-3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5.8763299648310497E-3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5.8763299648310497E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2.3191991032430101E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3.5254466740936002E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.59974789915966298</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.58549819927971103</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.58549819927971103</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.58549819927971103</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.95903961584633801</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.52965186074429704</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.71074925176279602</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.61904125158788503</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.61904125158788503</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.61904125158788503</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.92494221194879001</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.52215723563816396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.33639855942376901</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.44460984393757502</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.44460984393757502</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.44460984393757502</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.999159663865546</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.69877551020408102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.456659550543487</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.51752277681515801</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.51752277681515801</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.51752277681515801</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.96061956095196299</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.597691707397215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0.85871186561068202</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.72518379088681295</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.72518379088681295</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.72518379088681295</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0.85820577476293602</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0.35874738075789298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1.0319068118511E-2</v>
+      </c>
+      <c r="C22" s="10">
+        <v>7.1084687712042304E-3</v>
+      </c>
+      <c r="D22" s="10">
+        <v>7.1084687712042304E-3</v>
+      </c>
+      <c r="E22" s="10">
+        <v>7.1084687712042304E-3</v>
+      </c>
+      <c r="F22" s="10">
+        <v>2.5777289108789899E-2</v>
+      </c>
+      <c r="G22" s="10">
+        <v>4.40498218674915E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0.36794582392776498</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.49661399548532698</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.49661399548532698</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.49661399548532698</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0.95259593679458199</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0.720090293453724</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2.0075127778804099E-2</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1.40163098878695E-2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.40163098878695E-2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.40163098878695E-2</v>
+      </c>
+      <c r="F24" s="4">
+        <v>5.0196265017247499E-2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>8.7563991710242796E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.95542138472123606</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.87856354239448697</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.87856354239448697</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.87856354239448697</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.86435470880958298</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.24621711140386901</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4.7665607430945897E-3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.9144219729753599E-3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2.9144219729753599E-3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.9144219729753599E-3</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1.3862484157160901E-3</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.7658859096431399E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.15354330708661401</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.13779527559055099</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.98425196850393704</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2">
+        <v>9.2460881934566096E-3</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5.7641921397379899E-3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5.7641921397379899E-3</v>
+      </c>
+      <c r="E28" s="2">
+        <v>5.7641921397379899E-3</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2.7448827542937799E-3</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.5254466740936002E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.60264105642256904</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.58361344537815096</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.58361344537815096</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.58361344537815096</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.95895558223289301</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.52713085234093604</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.71389972981086702</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.61696839418264804</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.61696839418264804</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.61696839418264804</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.92487386366162105</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.52019732608850999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.34256902761104402</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.44103241296518603</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.44103241296518603</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.44103241296518603</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.99906362545018002</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.69877551020408102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.46297618275034003</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.51437212102544005</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.51437212102544005</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0.51437212102544005</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.96053831326969896</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0.596405664050492</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0.85959086550413699</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0.72566324537415205</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0.72566324537415205</v>
+      </c>
+      <c r="E35" s="10">
+        <v>0.72566324537415205</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0.85696274461057598</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0.35874738075789298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="10">
+        <v>1.0446525256385701E-2</v>
+      </c>
+      <c r="C36" s="10">
+        <v>7.0570716389887003E-3</v>
+      </c>
+      <c r="D36" s="10">
+        <v>7.0570716389887003E-3</v>
+      </c>
+      <c r="E36" s="10">
+        <v>7.0570716389887003E-3</v>
+      </c>
+      <c r="F36" s="10">
+        <v>2.5443751135881699E-2</v>
+      </c>
+      <c r="G36" s="10">
+        <v>4.40498218674915E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0.37020316027088002</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0.49209932279909702</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.49209932279909702</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0.49209932279909702</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.94808126410835203</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0.720090293453724</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2.0319662990955199E-2</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1.3914597561754E-2</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1.3914597561754E-2</v>
+      </c>
+      <c r="E38" s="4">
+        <v>1.3914597561754E-2</v>
+      </c>
+      <c r="F38" s="4">
+        <v>4.9557522123893798E-2</v>
+      </c>
+      <c r="G38" s="4">
+        <v>8.7563991710242796E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.74864658726645295</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.88047298774861404</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.88047298774861404</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.88047298774861404</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.86335198331635399</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.24621711140386901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.3147165003185302E-3</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2.9612347451543398E-3</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2.9612347451543398E-3</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2.9612347451543398E-3</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1.25835627211954E-3</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1.7658859096431399E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.429133858267716</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.25984251968503902</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.12598425196850299</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.98425196850393704</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="2">
+        <v>4.6045961473470702E-3</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5.85573595954218E-3</v>
+      </c>
+      <c r="D42" s="2">
+        <v>5.85573595954218E-3</v>
+      </c>
+      <c r="E42" s="2">
+        <v>5.85573595954218E-3</v>
+      </c>
+      <c r="F42" s="2">
+        <v>2.4918237034729702E-3</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3.5254466740936002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>